<commit_message>
bug fix, no need to give a range if we apply @ExcelCellRange.
</commit_message>
<xml_diff>
--- a/src/test/resources/test_multi.xlsx
+++ b/src/test/resources/test_multi.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ouokah-avae\Documents\SOCM\poiji\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hakan/IdeaProjects/p2o/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF17DA5A-570A-3A42-9660-FF550EEB43BE}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24000" windowHeight="9520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,26 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Age</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t>Class A</t>
   </si>
   <si>
-    <t>City</t>
-  </si>
-  <si>
-    <t>State</t>
-  </si>
-  <si>
-    <t>Zip Code</t>
-  </si>
-  <si>
     <t>Class B</t>
   </si>
   <si>
@@ -99,12 +85,42 @@
   </si>
   <si>
     <t>Washington</t>
+  </si>
+  <si>
+    <t>NameA</t>
+  </si>
+  <si>
+    <t>AgeA</t>
+  </si>
+  <si>
+    <t>CityA</t>
+  </si>
+  <si>
+    <t>StateA</t>
+  </si>
+  <si>
+    <t>Zip CodeA</t>
+  </si>
+  <si>
+    <t>NameB</t>
+  </si>
+  <si>
+    <t>AgeB</t>
+  </si>
+  <si>
+    <t>CityB</t>
+  </si>
+  <si>
+    <t>StateB</t>
+  </si>
+  <si>
+    <t>Zip CodeB</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -449,181 +465,181 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:J6"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>2</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>7</v>
       </c>
       <c r="B3">
         <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E3">
         <v>22349</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G3">
         <v>32</v>
       </c>
       <c r="H3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="I3" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="J3">
         <v>22309</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E4">
         <v>20993</v>
       </c>
       <c r="F4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G4">
         <v>25</v>
       </c>
       <c r="H4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="I4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="J4">
         <v>92384</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E5">
         <v>22312</v>
       </c>
       <c r="F5" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G5">
         <v>25</v>
       </c>
       <c r="H5" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="I5" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="J5">
         <v>22347</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B6">
         <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E6">
         <v>22314</v>
       </c>
       <c r="F6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G6">
         <v>35</v>
       </c>
       <c r="H6" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="I6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="J6">
         <v>90384</v>

</xml_diff>